<commit_message>
Auto commit at 2025-12-07  8:21:21.00
</commit_message>
<xml_diff>
--- a/chargingdata/202511-202511.xlsx
+++ b/chargingdata/202511-202511.xlsx
@@ -740,16 +740,61 @@
     <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -758,33 +803,45 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -798,6 +855,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -833,88 +899,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1224,7 +1224,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
@@ -1251,57 +1251,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="98"/>
+      <c r="M2" s="51"/>
     </row>
     <row r="3" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="101"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="54"/>
     </row>
     <row r="4" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="35" t="s">
@@ -1325,10 +1325,10 @@
       <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="84" t="s">
+      <c r="H4" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="83"/>
+      <c r="I4" s="47"/>
       <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1343,7 +1343,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="45" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1364,10 +1364,10 @@
       <c r="G5" s="3">
         <v>6440.87</v>
       </c>
-      <c r="H5" s="82">
+      <c r="H5" s="46">
         <v>8674</v>
       </c>
-      <c r="I5" s="83"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="35"/>
       <c r="K5" s="4">
         <v>2256.69</v>
@@ -1380,7 +1380,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="102"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="13" t="s">
         <v>33</v>
       </c>
@@ -1399,10 +1399,10 @@
       <c r="G6" s="3">
         <v>1919.55</v>
       </c>
-      <c r="H6" s="82">
+      <c r="H6" s="46">
         <v>2694</v>
       </c>
-      <c r="I6" s="83"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="35"/>
       <c r="K6" s="4">
         <v>690.84</v>
@@ -1415,7 +1415,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="102"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="13" t="s">
         <v>28</v>
       </c>
@@ -1434,10 +1434,10 @@
       <c r="G7" s="7">
         <v>125.5</v>
       </c>
-      <c r="H7" s="103">
+      <c r="H7" s="48">
         <v>162</v>
       </c>
-      <c r="I7" s="79"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="34"/>
       <c r="K7" s="4">
         <v>44.04</v>
@@ -1451,11 +1451,11 @@
       <c r="N7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="95"/>
-      <c r="C8" s="96"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="9">
         <v>270495.7</v>
       </c>
@@ -1468,10 +1468,10 @@
       <c r="G8" s="9">
         <v>8485.92</v>
       </c>
-      <c r="H8" s="89">
+      <c r="H8" s="59">
         <v>11530</v>
       </c>
-      <c r="I8" s="51"/>
+      <c r="I8" s="60"/>
       <c r="J8" s="41"/>
       <c r="K8" s="10">
         <v>2991.58</v>
@@ -1486,10 +1486,10 @@
       <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="63" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="35" t="s">
@@ -1507,10 +1507,10 @@
       <c r="G9" s="3">
         <v>852.03</v>
       </c>
-      <c r="H9" s="82">
+      <c r="H9" s="46">
         <v>1217</v>
       </c>
-      <c r="I9" s="83"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="35">
         <v>19.13</v>
       </c>
@@ -1527,8 +1527,8 @@
       <c r="P9" s="12"/>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="77"/>
-      <c r="B10" s="86"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="35" t="s">
         <v>37</v>
       </c>
@@ -1544,10 +1544,10 @@
       <c r="G10" s="3">
         <v>2494.0700000000002</v>
       </c>
-      <c r="H10" s="82">
+      <c r="H10" s="46">
         <v>3753</v>
       </c>
-      <c r="I10" s="83"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="35">
         <v>229.59</v>
       </c>
@@ -1565,11 +1565,11 @@
       <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="51"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="9">
         <v>135965.67000000001</v>
       </c>
@@ -1582,10 +1582,10 @@
       <c r="G11" s="9">
         <v>3346.1</v>
       </c>
-      <c r="H11" s="89">
+      <c r="H11" s="59">
         <v>4970</v>
       </c>
-      <c r="I11" s="51"/>
+      <c r="I11" s="60"/>
       <c r="J11" s="9">
         <v>248.72</v>
       </c>
@@ -1601,11 +1601,11 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="59"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="14">
         <v>406461.37</v>
       </c>
@@ -1618,10 +1618,10 @@
       <c r="G12" s="14">
         <v>11832.02</v>
       </c>
-      <c r="H12" s="90">
+      <c r="H12" s="71">
         <v>16500</v>
       </c>
-      <c r="I12" s="59"/>
+      <c r="I12" s="70"/>
       <c r="J12" s="14">
         <v>248.72</v>
       </c>
@@ -1637,30 +1637,30 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="92"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="92"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="92"/>
-      <c r="M13" s="93"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="74"/>
     </row>
     <row r="14" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="83"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="2" t="s">
         <v>41</v>
       </c>
@@ -1673,10 +1673,10 @@
       <c r="G14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="84" t="s">
+      <c r="H14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="83"/>
+      <c r="I14" s="47"/>
       <c r="J14" s="35" t="s">
         <v>46</v>
       </c>
@@ -1691,13 +1691,13 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="86"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="35">
         <v>230880</v>
       </c>
@@ -1710,10 +1710,10 @@
       <c r="G15" s="3">
         <v>25916.240000000002</v>
       </c>
-      <c r="H15" s="87">
+      <c r="H15" s="76">
         <v>863.87</v>
       </c>
-      <c r="I15" s="88"/>
+      <c r="I15" s="77"/>
       <c r="J15" s="18">
         <v>0.11219999999999999</v>
       </c>
@@ -1728,11 +1728,11 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="77"/>
-      <c r="B16" s="85" t="s">
+      <c r="A16" s="62"/>
+      <c r="B16" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="86"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="35">
         <v>70110</v>
       </c>
@@ -1745,10 +1745,10 @@
       <c r="G16" s="3">
         <v>8306.58</v>
       </c>
-      <c r="H16" s="87">
+      <c r="H16" s="76">
         <v>276.89</v>
       </c>
-      <c r="I16" s="88"/>
+      <c r="I16" s="77"/>
       <c r="J16" s="18">
         <v>0.11849999999999999</v>
       </c>
@@ -1764,11 +1764,11 @@
       <c r="O16" s="20"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="9">
         <v>300990</v>
       </c>
@@ -1781,10 +1781,10 @@
       <c r="G17" s="9">
         <v>34222.82</v>
       </c>
-      <c r="H17" s="55">
+      <c r="H17" s="66">
         <v>1140.76</v>
       </c>
-      <c r="I17" s="56"/>
+      <c r="I17" s="67"/>
       <c r="J17" s="21">
         <v>0.1137</v>
       </c>
@@ -1802,10 +1802,10 @@
       <c r="A18" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="51"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="41">
         <v>149850</v>
       </c>
@@ -1818,10 +1818,10 @@
       <c r="G18" s="9">
         <v>13884.33</v>
       </c>
-      <c r="H18" s="55">
+      <c r="H18" s="66">
         <v>462.81</v>
       </c>
-      <c r="I18" s="56"/>
+      <c r="I18" s="67"/>
       <c r="J18" s="21">
         <v>9.2700000000000005E-2</v>
       </c>
@@ -1836,11 +1836,11 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="59"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="14">
         <v>450840</v>
       </c>
@@ -1853,10 +1853,10 @@
       <c r="G19" s="14">
         <v>48107.15</v>
       </c>
-      <c r="H19" s="60">
+      <c r="H19" s="79">
         <v>1603.57</v>
       </c>
-      <c r="I19" s="61"/>
+      <c r="I19" s="80"/>
       <c r="J19" s="24">
         <v>0.1067</v>
       </c>
@@ -1871,30 +1871,30 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="63"/>
-      <c r="L20" s="63"/>
-      <c r="M20" s="64"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="83"/>
     </row>
     <row r="21" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="83"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="2" t="s">
         <v>55</v>
       </c>
@@ -1907,10 +1907,10 @@
       <c r="G21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="84" t="s">
+      <c r="H21" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="I21" s="83"/>
+      <c r="I21" s="47"/>
       <c r="J21" s="2" t="s">
         <v>60</v>
       </c>
@@ -1925,13 +1925,13 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="79"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="26">
         <v>2.13</v>
       </c>
@@ -1944,10 +1944,10 @@
       <c r="G22" s="26">
         <v>22.34</v>
       </c>
-      <c r="H22" s="80">
+      <c r="H22" s="85">
         <v>31.82</v>
       </c>
-      <c r="I22" s="81"/>
+      <c r="I22" s="86"/>
       <c r="J22" s="26">
         <v>2.86</v>
       </c>
@@ -1962,11 +1962,11 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A23" s="77"/>
-      <c r="B23" s="78" t="s">
+      <c r="A23" s="62"/>
+      <c r="B23" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="79"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="26">
         <v>2.67</v>
       </c>
@@ -1979,10 +1979,10 @@
       <c r="G23" s="26">
         <v>30.04</v>
       </c>
-      <c r="H23" s="80">
+      <c r="H23" s="85">
         <v>32.200000000000003</v>
       </c>
-      <c r="I23" s="81"/>
+      <c r="I23" s="86"/>
       <c r="J23" s="26">
         <v>3.9</v>
       </c>
@@ -1997,11 +1997,11 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="10">
         <v>2.21</v>
       </c>
@@ -2014,10 +2014,10 @@
       <c r="G24" s="10">
         <v>23.56</v>
       </c>
-      <c r="H24" s="55">
+      <c r="H24" s="66">
         <v>31.88</v>
       </c>
-      <c r="I24" s="56"/>
+      <c r="I24" s="67"/>
       <c r="J24" s="10">
         <v>3.03</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="A25" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="51"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="10">
         <v>3.1</v>
       </c>
@@ -2051,10 +2051,10 @@
       <c r="G25" s="10">
         <v>32.64</v>
       </c>
-      <c r="H25" s="55">
+      <c r="H25" s="66">
         <v>40.630000000000003</v>
       </c>
-      <c r="I25" s="56"/>
+      <c r="I25" s="67"/>
       <c r="J25" s="10">
         <v>4.5999999999999996</v>
       </c>
@@ -2069,11 +2069,11 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="58"/>
-      <c r="C26" s="59"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="70"/>
       <c r="D26" s="15">
         <v>2.4</v>
       </c>
@@ -2086,10 +2086,10 @@
       <c r="G26" s="15">
         <v>25.56</v>
       </c>
-      <c r="H26" s="60">
+      <c r="H26" s="79">
         <v>34.35</v>
       </c>
-      <c r="I26" s="61"/>
+      <c r="I26" s="80"/>
       <c r="J26" s="15">
         <v>3.37</v>
       </c>
@@ -2104,52 +2104,52 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A27" s="62" t="s">
+      <c r="A27" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="63"/>
-      <c r="M27" s="64"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="83"/>
     </row>
     <row r="28" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="71" t="s">
+      <c r="C28" s="90"/>
+      <c r="D28" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="73" t="s">
+      <c r="E28" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="73" t="s">
+      <c r="F28" s="96"/>
+      <c r="G28" s="96"/>
+      <c r="H28" s="96"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="L28" s="74"/>
-      <c r="M28" s="75"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="97"/>
     </row>
     <row r="29" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A29" s="66"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="72"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="94"/>
       <c r="E29" s="31" t="s">
         <v>70</v>
       </c>
@@ -2179,13 +2179,13 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="47"/>
+      <c r="C30" s="100"/>
       <c r="D30" s="3">
         <v>181648.89</v>
       </c>
@@ -2219,11 +2219,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A31" s="46"/>
-      <c r="B31" s="47" t="s">
+      <c r="A31" s="99"/>
+      <c r="B31" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="47"/>
+      <c r="C31" s="100"/>
       <c r="D31" s="3">
         <v>54801.8</v>
       </c>
@@ -2257,11 +2257,11 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A32" s="46"/>
-      <c r="B32" s="48" t="s">
+      <c r="A32" s="99"/>
+      <c r="B32" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="47"/>
+      <c r="C32" s="100"/>
       <c r="D32" s="3">
         <v>3119.66</v>
       </c>
@@ -2295,11 +2295,11 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="51"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="9">
         <v>239570.35</v>
       </c>
@@ -2336,10 +2336,10 @@
       <c r="A34" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="52" t="s">
+      <c r="B34" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="53"/>
+      <c r="C34" s="103"/>
       <c r="D34" s="9">
         <v>118954.65</v>
       </c>
@@ -2373,11 +2373,11 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
       <c r="D35" s="14">
         <v>358525</v>
       </c>
@@ -2413,21 +2413,37 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A20:M20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H23:I23"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="A11:C11"/>
@@ -2442,37 +2458,21 @@
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:M27"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>